<commit_message>
Update Cahier de Test version3.xlsx
</commit_message>
<xml_diff>
--- a/V3/Cahier de Test version3.xlsx
+++ b/V3/Cahier de Test version3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthurchauvel/Desktop/cours/SAES/S101/V3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E38F38-7AE3-CA45-893F-F2A414BE9EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20A6D0B-78E0-E847-B011-31A8E8525475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="34200" windowHeight="21400" xr2:uid="{2AC9D963-C8E2-174A-A134-F330AB6D3BF7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34200" windowHeight="21100" xr2:uid="{2AC9D963-C8E2-174A-A134-F330AB6D3BF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -194,31 +194,31 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,7 +537,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -549,10 +549,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="50" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
@@ -560,10 +560,10 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="50" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
@@ -571,10 +571,10 @@
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="50" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
@@ -582,112 +582,115 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="18">
-      <c r="A4" s="6"/>
+      <c r="A4" s="4"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" ht="50" customHeight="1">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="50" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="50" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="50" customHeight="1">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="50" customHeight="1">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="51" customHeight="1">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="11" spans="1:5" ht="33" customHeight="1">
+      <c r="A11" s="6"/>
     </row>
     <row r="17" customFormat="1"/>
   </sheetData>

</xml_diff>